<commit_message>
form for account funding created
</commit_message>
<xml_diff>
--- a/Excels/BuySell.xlsx
+++ b/Excels/BuySell.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="14925" windowHeight="2865"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="14925" windowHeight="2865" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Buy Order" sheetId="1" r:id="rId1"/>
     <sheet name="Sell Order" sheetId="2" r:id="rId2"/>
+    <sheet name="Account Funding Deposit" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Cost</t>
   </si>
@@ -34,6 +35,15 @@
   </si>
   <si>
     <t>Expiry</t>
+  </si>
+  <si>
+    <t>private key</t>
+  </si>
+  <si>
+    <t>amount to deposit</t>
+  </si>
+  <si>
+    <t>fe1ef34ed4476ec0e7fabb2388d4a0e258d2ab28401a9836de60fcd44eb267b0</t>
   </si>
 </sst>
 </file>
@@ -396,7 +406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -490,4 +500,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
xml test file for buysell order is added
</commit_message>
<xml_diff>
--- a/Excels/BuySell.xlsx
+++ b/Excels/BuySell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="14925" windowHeight="2865" activeTab="3"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="14925" windowHeight="2865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Buy Order" sheetId="1" r:id="rId1"/>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,24 +439,585 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -466,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,24 +1048,607 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -551,7 +1695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>